<commit_message>
Add keyboard tracker and SQLite
</commit_message>
<xml_diff>
--- a/data/ledger.xlsx
+++ b/data/ledger.xlsx
@@ -642,7 +642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1239,6 +1239,111 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>печать (1).docx</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2025-06-26 07:59:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ee71121c452ebe95882145ee5a20077b.pdf</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2025-06-26 12:26:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>b40d26a2f26fd1f152f53ad626929df7.pdf</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2025-06-26 13:12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>746382370</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Курсовая Прашкович.docx</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2025-06-26 14:59:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>печать.pdf</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>14</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2025-06-26 19:56:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add shell, ban, ping
</commit_message>
<xml_diff>
--- a/data/ledger.xlsx
+++ b/data/ledger.xlsx
@@ -642,7 +642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1365,6 +1365,27 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>M-Банкинг чек-4294968789.docx</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2025-06-28 01:33:45</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add print options UI
</commit_message>
<xml_diff>
--- a/data/ledger.xlsx
+++ b/data/ledger.xlsx
@@ -642,7 +642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1386,6 +1386,153 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>M-Банкинг чек-4294968802.pdf</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2025-06-28 14:22:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ПЕЧАТЬ11.docx</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>2</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2025-06-28 14:23:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>M-Банкинг чек-4294968802.pdf</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2025-06-28 14:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>M-Банкинг чек-4294968802.pdf</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2025-06-28 14:23:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>M-Банкинг чек-4294968802.pdf</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2025-06-28 14:25:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>357d1a45e0e15379ea555a7e8964ca76.pdf</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2025-06-28 14:29:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>M-Банкинг чек.docx</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2025-06-28 14:33:43</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add ensure_data decorator, layout options. Ref: decorators moved to modules/decorators.py.
</commit_message>
<xml_diff>
--- a/data/ledger.xlsx
+++ b/data/ledger.xlsx
@@ -642,7 +642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1533,6 +1533,48 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>M-Банкинг чек-4294968802.pdf</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2025-06-28 20:15:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>M-Банкинг чек-4294968802.pdf</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2025-06-28 20:16:28</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add copies option, ref other options
</commit_message>
<xml_diff>
--- a/data/ledger.xlsx
+++ b/data/ledger.xlsx
@@ -642,7 +642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1722,6 +1722,342 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>6, 7.docx</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>4</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2025-07-07 01:17:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>6, 7.docx</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>4</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2025-07-07 01:18:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>6, 7.docx</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>4</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2025-07-07 01:19:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>6, 7.docx</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2025-07-07 01:25:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>3.docx</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>2</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2025-07-07 01:46:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>6, 7.docx</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>4</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2025-07-07 01:47:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>debug.pdf</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>4</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:07:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>debug.pdf</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>4</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:09:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>debug.pdf</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>4</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:11:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>debug.pdf</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>4</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:34:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>debug.pdf</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>4</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:47:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>debug.pdf</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:49:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Radkovich_Otchetik.docx</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>33</v>
+      </c>
+      <c r="D64" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:51:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Radkovich_Otchetik.docx</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>33</v>
+      </c>
+      <c r="D65" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:54:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Radkovich_Otchetik.docx</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>33</v>
+      </c>
+      <c r="D66" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:54:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Radkovich_Otchetik.docx</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>33</v>
+      </c>
+      <c r="D67" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2025-07-09 15:57:15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove users module, ref Admin, add Promo creation, fix pages rotation
</commit_message>
<xml_diff>
--- a/data/ledger.xlsx
+++ b/data/ledger.xlsx
@@ -642,7 +642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2058,6 +2058,447 @@
         </is>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Ходатайство студенты 2025.docx</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>3</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2025-07-11 21:49:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Ходатайство студенты 2025.docx</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>3</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2025-07-11 21:54:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Ходатайство студенты 2025.docx</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>3</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2025-07-11 21:56:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Ходатайство студенты 2025.docx</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>3</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2025-07-11 22:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>40</v>
+      </c>
+      <c r="D72" t="n">
+        <v>8</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2025-07-11 22:01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>40</v>
+      </c>
+      <c r="D73" t="n">
+        <v>8</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2025-07-11 22:15:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>40</v>
+      </c>
+      <c r="D74" t="n">
+        <v>8</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2025-07-11 22:23:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>40</v>
+      </c>
+      <c r="D75" t="n">
+        <v>8</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2025-07-11 22:25:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>40</v>
+      </c>
+      <c r="D76" t="n">
+        <v>8</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2025-07-11 22:34:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>40</v>
+      </c>
+      <c r="D77" t="n">
+        <v>8</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2025-07-11 22:38:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>40</v>
+      </c>
+      <c r="D78" t="n">
+        <v>8</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2025-07-11 22:58:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>40</v>
+      </c>
+      <c r="D79" t="n">
+        <v>8</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:00:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>40</v>
+      </c>
+      <c r="D80" t="n">
+        <v>8</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:03:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>40</v>
+      </c>
+      <c r="D81" t="n">
+        <v>8</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:11:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>40</v>
+      </c>
+      <c r="D82" t="n">
+        <v>8</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:17:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>40</v>
+      </c>
+      <c r="D83" t="n">
+        <v>8</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:34:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>40</v>
+      </c>
+      <c r="D84" t="n">
+        <v>8</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:36:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>40</v>
+      </c>
+      <c r="D85" t="n">
+        <v>8</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:41:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>40</v>
+      </c>
+      <c r="D86" t="n">
+        <v>8</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:44:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>40</v>
+      </c>
+      <c r="D87" t="n">
+        <v>8</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:45:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>7676096317</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>отчет маз 9docx.pdf</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>40</v>
+      </c>
+      <c r="D88" t="n">
+        <v>8</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2025-07-11 23:49:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>